<commit_message>
parts now care about what is next to them!
</commit_message>
<xml_diff>
--- a/partslist/sourceplate4.xlsx
+++ b/partslist/sourceplate4.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Documents\GitHub\makeMocloAssy\partslist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\makeMocloAssy\partslist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="11_EC8063478EBF936FFD54A2F8C57FAD2ACB3C7DE7" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{861006ED-365E-464F-8C79-344CAE70A10C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10800" windowWidth="22125" windowHeight="1260" tabRatio="799" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="22125" windowHeight="1260" tabRatio="799"/>
   </bookViews>
   <sheets>
     <sheet name="parts_1" sheetId="10" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Gibson!$A$1:$P$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parts_1!$A$1:$O$175</definedName>
   </definedNames>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="830">
   <si>
     <t>well</t>
   </si>
@@ -2517,12 +2516,18 @@
   </si>
   <si>
     <t xml:space="preserve">ECK120033736 (164.6x), short attachment </t>
+  </si>
+  <si>
+    <t>strongWeissRBS2</t>
+  </si>
+  <si>
+    <t>T2m2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2628,8 +2633,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2909,27 +2914,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="J122" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="R135" sqref="R135"/>
+      <selection pane="bottomLeft" activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.484375" customWidth="1"/>
-    <col min="3" max="3" width="39.14453125" customWidth="1"/>
-    <col min="4" max="4" width="9.953125" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.203125" customWidth="1"/>
-    <col min="10" max="10" width="36.58984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2979,7 +2984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3031,7 +3036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -3083,7 +3088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -3135,7 +3140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3187,7 +3192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -3291,7 +3296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -3343,7 +3348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -3395,7 +3400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -3447,7 +3452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3499,7 +3504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -3551,7 +3556,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -3655,7 +3660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -3707,7 +3712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -3759,7 +3764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -3811,7 +3816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -3863,7 +3868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -3915,7 +3920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -3967,7 +3972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -4019,7 +4024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -4071,7 +4076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -4123,7 +4128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -4175,7 +4180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -4227,7 +4232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -4279,7 +4284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -4331,7 +4336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4383,7 +4388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -4435,7 +4440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -4539,7 +4544,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -4591,7 +4596,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -4643,7 +4648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -4695,7 +4700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -4747,7 +4752,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -4799,7 +4804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>176</v>
       </c>
@@ -4851,7 +4856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>180</v>
       </c>
@@ -4903,7 +4908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -4955,7 +4960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>188</v>
       </c>
@@ -5007,7 +5012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -5059,7 +5064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -5111,7 +5116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>200</v>
       </c>
@@ -5163,7 +5168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>204</v>
       </c>
@@ -5215,7 +5220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -5267,7 +5272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>212</v>
       </c>
@@ -5319,7 +5324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>218</v>
       </c>
@@ -5371,7 +5376,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>222</v>
       </c>
@@ -5423,7 +5428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>226</v>
       </c>
@@ -5475,7 +5480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>230</v>
       </c>
@@ -5527,7 +5532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>234</v>
       </c>
@@ -5579,7 +5584,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>238</v>
       </c>
@@ -5631,7 +5636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>242</v>
       </c>
@@ -5683,7 +5688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>246</v>
       </c>
@@ -5731,7 +5736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>250</v>
       </c>
@@ -5779,7 +5784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -5827,7 +5832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>258</v>
       </c>
@@ -5875,7 +5880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>261</v>
       </c>
@@ -5923,7 +5928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>264</v>
       </c>
@@ -5971,7 +5976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>267</v>
       </c>
@@ -6019,7 +6024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>270</v>
       </c>
@@ -6067,7 +6072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>273</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>277</v>
       </c>
@@ -6171,7 +6176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>281</v>
       </c>
@@ -6223,7 +6228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>285</v>
       </c>
@@ -6269,7 +6274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>289</v>
       </c>
@@ -6315,7 +6320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>292</v>
       </c>
@@ -6361,7 +6366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>295</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>297</v>
       </c>
@@ -6453,7 +6458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>301</v>
       </c>
@@ -6499,7 +6504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>304</v>
       </c>
@@ -6545,7 +6550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>307</v>
       </c>
@@ -6597,7 +6602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>311</v>
       </c>
@@ -6646,7 +6651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>314</v>
       </c>
@@ -6695,7 +6700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>316</v>
       </c>
@@ -6744,7 +6749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>318</v>
       </c>
@@ -6793,7 +6798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>320</v>
       </c>
@@ -6842,7 +6847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>322</v>
       </c>
@@ -6891,7 +6896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>324</v>
       </c>
@@ -6936,7 +6941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>329</v>
       </c>
@@ -6981,7 +6986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>331</v>
       </c>
@@ -7026,7 +7031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>333</v>
       </c>
@@ -7071,7 +7076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>335</v>
       </c>
@@ -7116,7 +7121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>337</v>
       </c>
@@ -7161,7 +7166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>339</v>
       </c>
@@ -7206,7 +7211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>341</v>
       </c>
@@ -7251,12 +7256,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>343</v>
       </c>
       <c r="B87" t="s">
-        <v>209</v>
+        <v>828</v>
       </c>
       <c r="C87" t="s">
         <v>210</v>
@@ -7303,7 +7308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>344</v>
       </c>
@@ -7355,7 +7360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>348</v>
       </c>
@@ -7404,7 +7409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>352</v>
       </c>
@@ -7456,7 +7461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>355</v>
       </c>
@@ -7505,7 +7510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>359</v>
       </c>
@@ -7554,7 +7559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>363</v>
       </c>
@@ -7603,7 +7608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>367</v>
       </c>
@@ -7652,7 +7657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>371</v>
       </c>
@@ -7701,7 +7706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>374</v>
       </c>
@@ -7750,7 +7755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>377</v>
       </c>
@@ -7799,7 +7804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>380</v>
       </c>
@@ -7848,7 +7853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>384</v>
       </c>
@@ -7897,7 +7902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>388</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>392</v>
       </c>
@@ -7995,7 +8000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>396</v>
       </c>
@@ -8044,7 +8049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>400</v>
       </c>
@@ -8093,7 +8098,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>404</v>
       </c>
@@ -8142,7 +8147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>408</v>
       </c>
@@ -8191,7 +8196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>412</v>
       </c>
@@ -8240,7 +8245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>416</v>
       </c>
@@ -8292,7 +8297,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>420</v>
       </c>
@@ -8344,7 +8349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>423</v>
       </c>
@@ -8366,7 +8371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>464</v>
       </c>
@@ -8418,7 +8423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>468</v>
       </c>
@@ -8470,7 +8475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>472</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>476</v>
       </c>
@@ -8574,7 +8579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>480</v>
       </c>
@@ -8626,7 +8631,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>484</v>
       </c>
@@ -8678,7 +8683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>488</v>
       </c>
@@ -8730,7 +8735,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>491</v>
       </c>
@@ -8782,7 +8787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>494</v>
       </c>
@@ -8834,7 +8839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>497</v>
       </c>
@@ -8886,7 +8891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>500</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>533</v>
       </c>
@@ -8987,7 +8992,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>536</v>
       </c>
@@ -9039,7 +9044,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>540</v>
       </c>
@@ -9091,7 +9096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>543</v>
       </c>
@@ -9143,7 +9148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>546</v>
       </c>
@@ -9195,7 +9200,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>549</v>
       </c>
@@ -9247,7 +9252,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>552</v>
       </c>
@@ -9299,7 +9304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>555</v>
       </c>
@@ -9351,7 +9356,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>558</v>
       </c>
@@ -9403,7 +9408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>562</v>
       </c>
@@ -9455,7 +9460,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>566</v>
       </c>
@@ -9507,7 +9512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>569</v>
       </c>
@@ -9559,7 +9564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>572</v>
       </c>
@@ -9611,7 +9616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>575</v>
       </c>
@@ -9663,7 +9668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>579</v>
       </c>
@@ -9715,7 +9720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>582</v>
       </c>
@@ -9767,7 +9772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>585</v>
       </c>
@@ -9819,7 +9824,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>588</v>
       </c>
@@ -9871,7 +9876,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>591</v>
       </c>
@@ -9923,7 +9928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>594</v>
       </c>
@@ -9975,7 +9980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>824</v>
       </c>
@@ -10023,12 +10028,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>825</v>
       </c>
       <c r="B142" t="s">
-        <v>164</v>
+        <v>829</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>827</v>
@@ -10051,7 +10056,7 @@
       <c r="I142" s="12">
         <v>7103</v>
       </c>
-      <c r="J142" s="14" t="s">
+      <c r="J142" s="13" t="s">
         <v>167</v>
       </c>
       <c r="K142" s="12" t="b">
@@ -10074,43 +10079,43 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H143" s="3"/>
       <c r="O143" s="4"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H144" s="3"/>
       <c r="O144" s="4"/>
     </row>
-    <row r="145" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H145" s="3"/>
       <c r="O145" s="4"/>
     </row>
-    <row r="146" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H146" s="3"/>
       <c r="O146" s="4"/>
     </row>
-    <row r="147" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H147" s="3"/>
       <c r="O147" s="4"/>
     </row>
-    <row r="148" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H148" s="3"/>
       <c r="O148" s="4"/>
     </row>
-    <row r="149" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H149" s="3"/>
       <c r="O149" s="4"/>
     </row>
-    <row r="150" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H150" s="3"/>
       <c r="O150" s="4"/>
     </row>
-    <row r="151" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H151" s="3"/>
       <c r="O151" s="4"/>
     </row>
-    <row r="152" spans="3:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -10124,7 +10129,7 @@
       <c r="N152" s="4"/>
       <c r="O152" s="4"/>
     </row>
-    <row r="153" spans="3:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -10138,7 +10143,7 @@
       <c r="N153" s="4"/>
       <c r="O153" s="4"/>
     </row>
-    <row r="154" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -10152,7 +10157,7 @@
       <c r="N154" s="4"/>
       <c r="O154" s="4"/>
     </row>
-    <row r="155" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -10166,7 +10171,7 @@
       <c r="N155" s="4"/>
       <c r="O155" s="4"/>
     </row>
-    <row r="156" spans="3:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -10180,7 +10185,7 @@
       <c r="N156" s="4"/>
       <c r="O156" s="4"/>
     </row>
-    <row r="157" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -10194,7 +10199,7 @@
       <c r="N157" s="4"/>
       <c r="O157" s="4"/>
     </row>
-    <row r="158" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -10208,7 +10213,7 @@
       <c r="N158" s="4"/>
       <c r="O158" s="4"/>
     </row>
-    <row r="159" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
@@ -10221,7 +10226,7 @@
       <c r="N159" s="4"/>
       <c r="O159" s="4"/>
     </row>
-    <row r="160" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
       <c r="F160" s="4"/>
@@ -10233,7 +10238,7 @@
       <c r="N160" s="4"/>
       <c r="O160" s="4"/>
     </row>
-    <row r="161" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
       <c r="F161" s="4"/>
@@ -10245,54 +10250,54 @@
       <c r="N161" s="4"/>
       <c r="O161" s="4"/>
     </row>
-    <row r="162" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H162" s="3"/>
       <c r="O162" s="4"/>
     </row>
-    <row r="163" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H163" s="3"/>
       <c r="O163" s="4"/>
     </row>
-    <row r="164" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H164" s="3"/>
       <c r="O164" s="4"/>
     </row>
-    <row r="165" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H165" s="3"/>
       <c r="O165" s="4"/>
     </row>
-    <row r="166" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O166" s="4"/>
     </row>
-    <row r="167" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O167" s="4"/>
     </row>
-    <row r="168" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O168" s="4"/>
     </row>
-    <row r="169" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O169" s="4"/>
     </row>
-    <row r="170" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O170" s="4"/>
     </row>
-    <row r="171" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O171" s="4"/>
     </row>
-    <row r="172" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O172" s="4"/>
     </row>
-    <row r="173" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O173" s="4"/>
     </row>
-    <row r="174" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O174" s="4"/>
     </row>
-    <row r="175" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:15" x14ac:dyDescent="0.25">
       <c r="O175" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O175" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:O175">
     <sortState ref="A2:O197">
       <sortCondition ref="I1:I197"/>
     </sortState>
@@ -10393,7 +10398,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92 G94">
+  <conditionalFormatting sqref="G94 G92">
     <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
@@ -10555,25 +10560,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.2578125" customWidth="1"/>
-    <col min="3" max="3" width="9.14453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.4375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10623,7 +10628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -10663,7 +10668,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>429</v>
       </c>
@@ -10697,7 +10702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -10737,7 +10742,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -10777,7 +10782,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -10817,7 +10822,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>450</v>
       </c>
@@ -10851,7 +10856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>453</v>
       </c>
@@ -10885,7 +10890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>456</v>
       </c>
@@ -10919,7 +10924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>620</v>
       </c>
@@ -10953,7 +10958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>623</v>
       </c>
@@ -10996,7 +11001,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>628</v>
       </c>
@@ -11039,7 +11044,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>631</v>
       </c>
@@ -11082,7 +11087,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>634</v>
       </c>
@@ -11125,7 +11130,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>637</v>
       </c>
@@ -11168,7 +11173,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>640</v>
       </c>
@@ -11211,7 +11216,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>643</v>
       </c>
@@ -11254,7 +11259,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>646</v>
       </c>
@@ -11297,7 +11302,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>649</v>
       </c>
@@ -11340,7 +11345,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>652</v>
       </c>
@@ -11383,7 +11388,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>656</v>
       </c>
@@ -11426,7 +11431,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>659</v>
       </c>
@@ -11469,7 +11474,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>662</v>
       </c>
@@ -11512,7 +11517,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>665</v>
       </c>
@@ -11555,7 +11560,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>668</v>
       </c>
@@ -11598,7 +11603,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>671</v>
       </c>
@@ -11641,7 +11646,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>674</v>
       </c>
@@ -11684,7 +11689,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>677</v>
       </c>
@@ -11722,7 +11727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>681</v>
       </c>
@@ -11762,7 +11767,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>684</v>
       </c>
@@ -11802,7 +11807,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>687</v>
       </c>
@@ -11842,7 +11847,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>690</v>
       </c>
@@ -11882,7 +11887,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>693</v>
       </c>
@@ -11922,7 +11927,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>696</v>
       </c>
@@ -11962,7 +11967,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>699</v>
       </c>
@@ -12002,7 +12007,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>702</v>
       </c>
@@ -12042,7 +12047,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>705</v>
       </c>
@@ -12082,7 +12087,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>708</v>
       </c>
@@ -12122,7 +12127,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>711</v>
       </c>
@@ -12162,7 +12167,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>714</v>
       </c>
@@ -12202,7 +12207,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>717</v>
       </c>
@@ -12242,7 +12247,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>720</v>
       </c>
@@ -12282,7 +12287,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -12320,7 +12325,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -12358,7 +12363,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -12396,7 +12401,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>118</v>
       </c>
@@ -12434,7 +12439,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -12472,7 +12477,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>733</v>
       </c>
@@ -12504,7 +12509,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>734</v>
       </c>
@@ -12536,7 +12541,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>735</v>
       </c>
@@ -12568,7 +12573,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>736</v>
       </c>
@@ -12600,7 +12605,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -12638,7 +12643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -12676,7 +12681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -12714,7 +12719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -12752,7 +12757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -12790,7 +12795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -12828,7 +12833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -12866,7 +12871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -12904,7 +12909,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -12942,7 +12947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -12989,7 +12994,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -13036,7 +13041,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -13083,7 +13088,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>35</v>
       </c>
@@ -13130,7 +13135,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -13177,7 +13182,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>44</v>
       </c>
@@ -13224,7 +13229,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -13271,7 +13276,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -13318,7 +13323,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -13365,7 +13370,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -13412,7 +13417,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -13459,7 +13464,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -13506,7 +13511,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -13553,7 +13558,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -13600,7 +13605,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -13647,17 +13652,17 @@
         <v>601</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="D76" s="13"/>
+      <c r="D76" s="14"/>
       <c r="E76" t="str">
         <f t="shared" ref="E76:E79" si="9">"UNS"&amp;LEFT(RIGHT(B76,3),1)</f>
         <v>UNS5</v>
@@ -13694,17 +13699,17 @@
         <v>601</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>787</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="D77" s="13"/>
+      <c r="D77" s="14"/>
       <c r="E77" t="str">
         <f t="shared" si="9"/>
         <v>UNS4</v>
@@ -13741,17 +13746,17 @@
         <v>601</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>789</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="D78" s="13"/>
+      <c r="D78" s="14"/>
       <c r="E78" t="str">
         <f t="shared" si="9"/>
         <v>UNS5</v>
@@ -13788,17 +13793,17 @@
         <v>601</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>791</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="D79" s="13"/>
+      <c r="D79" s="14"/>
       <c r="E79" t="str">
         <f t="shared" si="9"/>
         <v>UNS4</v>
@@ -13835,7 +13840,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>143</v>
       </c>
@@ -13878,7 +13883,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>148</v>
       </c>
@@ -13921,7 +13926,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>152</v>
       </c>
@@ -13965,7 +13970,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P82" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:P82"/>
   <mergeCells count="4">
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
@@ -14277,16 +14282,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14336,7 +14341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>425</v>
       </c>
@@ -14379,7 +14384,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>429</v>
       </c>
@@ -14422,7 +14427,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>432</v>
       </c>
@@ -14465,7 +14470,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>435</v>
       </c>
@@ -14508,7 +14513,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -14551,7 +14556,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>441</v>
       </c>
@@ -14591,7 +14596,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>444</v>
       </c>
@@ -14631,7 +14636,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>447</v>
       </c>
@@ -14673,7 +14678,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>450</v>
       </c>
@@ -14715,7 +14720,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>453</v>
       </c>
@@ -14757,7 +14762,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>456</v>
       </c>
@@ -14809,7 +14814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>460</v>
       </c>
@@ -14861,7 +14866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>504</v>
       </c>
@@ -14895,7 +14900,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>507</v>
       </c>
@@ -14929,7 +14934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>510</v>
       </c>
@@ -14963,7 +14968,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>513</v>
       </c>
@@ -14997,7 +15002,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>516</v>
       </c>
@@ -15031,7 +15036,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>516</v>
       </c>
@@ -15065,7 +15070,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>521</v>
       </c>
@@ -15099,7 +15104,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>524</v>
       </c>
@@ -15133,7 +15138,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>527</v>
       </c>
@@ -15167,7 +15172,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>530</v>
       </c>
@@ -15351,16 +15356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>798</v>
       </c>
@@ -15371,7 +15376,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>801</v>
       </c>
@@ -15382,7 +15387,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>801</v>
       </c>
@@ -15393,7 +15398,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>804</v>
       </c>
@@ -15404,7 +15409,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>805</v>
       </c>
@@ -15415,7 +15420,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>804</v>
       </c>
@@ -15426,7 +15431,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>805</v>
       </c>
@@ -15443,17 +15448,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -15527,7 +15532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -15604,7 +15609,7 @@
         <v>31.85</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -15681,7 +15686,7 @@
         <v>31.49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -15758,7 +15763,7 @@
         <v>33.19</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -15835,7 +15840,7 @@
         <v>32.369999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -15912,7 +15917,7 @@
         <v>32.090000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -15989,7 +15994,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>327</v>
       </c>
@@ -16066,7 +16071,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>807</v>
       </c>
@@ -16143,7 +16148,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -16220,7 +16225,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>808</v>
       </c>
@@ -16297,7 +16302,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>809</v>
       </c>
@@ -16374,7 +16379,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>810</v>
       </c>
@@ -16451,7 +16456,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>811</v>
       </c>
@@ -16528,7 +16533,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>812</v>
       </c>
@@ -16605,7 +16610,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>813</v>
       </c>
@@ -16682,7 +16687,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>814</v>
       </c>

</xml_diff>

<commit_message>
fixed date on parts
</commit_message>
<xml_diff>
--- a/partslist/sourceplate4.xlsx
+++ b/partslist/sourceplate4.xlsx
@@ -10557,7 +10557,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92 G94">
+  <conditionalFormatting sqref="G94 G92">
     <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
@@ -10724,9 +10724,9 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13507,7 +13507,7 @@
         <v>30</v>
       </c>
       <c r="H56" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I56">
         <f t="shared" si="2"/>
@@ -13558,7 +13558,7 @@
         <v>30</v>
       </c>
       <c r="H57" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I57">
         <f t="shared" si="2"/>
@@ -13609,7 +13609,7 @@
         <v>30</v>
       </c>
       <c r="H58" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I58">
         <f t="shared" si="2"/>
@@ -13660,7 +13660,7 @@
         <v>30</v>
       </c>
       <c r="H59" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I59">
         <f t="shared" si="2"/>
@@ -13711,7 +13711,7 @@
         <v>30</v>
       </c>
       <c r="H60" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I60">
         <f t="shared" si="2"/>
@@ -13762,7 +13762,7 @@
         <v>30</v>
       </c>
       <c r="H61" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I61">
         <f t="shared" si="2"/>
@@ -13813,7 +13813,7 @@
         <v>30</v>
       </c>
       <c r="H62" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I62">
         <f t="shared" si="2"/>
@@ -13864,7 +13864,7 @@
         <v>30</v>
       </c>
       <c r="H63" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I63">
         <f t="shared" si="2"/>
@@ -13915,7 +13915,7 @@
         <v>30</v>
       </c>
       <c r="H64" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I64">
         <f t="shared" si="2"/>
@@ -13966,7 +13966,7 @@
         <v>30</v>
       </c>
       <c r="H65" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I65">
         <f t="shared" si="2"/>
@@ -14017,7 +14017,7 @@
         <v>30</v>
       </c>
       <c r="H66" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I66">
         <f t="shared" si="2"/>
@@ -14068,7 +14068,7 @@
         <v>30</v>
       </c>
       <c r="H67" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I67">
         <f t="shared" ref="I67" si="18">CODE(LEFT(A67,1))*100+MID(A67,2,10)</f>
@@ -14119,7 +14119,7 @@
         <v>30</v>
       </c>
       <c r="H68" s="3">
-        <v>43301</v>
+        <v>43304</v>
       </c>
       <c r="I68">
         <f>CODE(LEFT(A68,1))*100+MID(A68,2,10)</f>

</xml_diff>

<commit_message>
added ability to make new columns and progress bar
</commit_message>
<xml_diff>
--- a/partslist/sourceplate4.xlsx
+++ b/partslist/sourceplate4.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="882">
   <si>
     <t>well</t>
   </si>
@@ -10557,7 +10557,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G94 G92">
+  <conditionalFormatting sqref="G92 G94">
     <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
@@ -10721,12 +10721,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
+      <selection pane="bottomLeft" activeCell="P78" sqref="P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13504,7 +13504,7 @@
         <v>UNS6</v>
       </c>
       <c r="G56">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H56" s="3">
         <v>43304</v>
@@ -13555,7 +13555,7 @@
         <v>UNS6</v>
       </c>
       <c r="G57">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H57" s="3">
         <v>43304</v>
@@ -13606,7 +13606,7 @@
         <v>UNS5</v>
       </c>
       <c r="G58">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H58" s="3">
         <v>43304</v>
@@ -13657,7 +13657,7 @@
         <v>UNS6</v>
       </c>
       <c r="G59">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H59" s="3">
         <v>43304</v>
@@ -13708,7 +13708,7 @@
         <v>UNS6</v>
       </c>
       <c r="G60">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H60" s="3">
         <v>43304</v>
@@ -13759,7 +13759,7 @@
         <v>UNS5</v>
       </c>
       <c r="G61">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H61" s="3">
         <v>43304</v>
@@ -13810,7 +13810,7 @@
         <v>UNS3</v>
       </c>
       <c r="G62">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H62" s="3">
         <v>43304</v>
@@ -13861,7 +13861,7 @@
         <v>UNS3</v>
       </c>
       <c r="G63">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H63" s="3">
         <v>43304</v>
@@ -13912,7 +13912,7 @@
         <v>UNSX</v>
       </c>
       <c r="G64">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H64" s="3">
         <v>43304</v>
@@ -13963,7 +13963,7 @@
         <v>UNS5</v>
       </c>
       <c r="G65">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H65" s="3">
         <v>43304</v>
@@ -14014,7 +14014,7 @@
         <v>UNS7</v>
       </c>
       <c r="G66">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H66" s="3">
         <v>43304</v>
@@ -14065,7 +14065,7 @@
         <v>UNS7</v>
       </c>
       <c r="G67">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H67" s="3">
         <v>43304</v>
@@ -14116,7 +14116,7 @@
         <v>UNS7</v>
       </c>
       <c r="G68">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H68" s="3">
         <v>43304</v>
@@ -14145,6 +14145,869 @@
         <v>600</v>
       </c>
       <c r="P68" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>622</v>
+      </c>
+      <c r="B69" t="s">
+        <v>623</v>
+      </c>
+      <c r="C69" t="s">
+        <v>624</v>
+      </c>
+      <c r="D69" t="s">
+        <v>625</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" t="s">
+        <v>47</v>
+      </c>
+      <c r="G69">
+        <v>30</v>
+      </c>
+      <c r="H69" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J69" t="s">
+        <v>626</v>
+      </c>
+      <c r="K69" t="b">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>379</v>
+      </c>
+      <c r="O69" t="s">
+        <v>600</v>
+      </c>
+      <c r="P69" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>627</v>
+      </c>
+      <c r="B70" t="s">
+        <v>628</v>
+      </c>
+      <c r="C70" t="s">
+        <v>624</v>
+      </c>
+      <c r="D70" t="s">
+        <v>625</v>
+      </c>
+      <c r="E70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70">
+        <v>30</v>
+      </c>
+      <c r="H70" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J70" t="s">
+        <v>629</v>
+      </c>
+      <c r="K70" t="b">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>379</v>
+      </c>
+      <c r="O70" t="s">
+        <v>600</v>
+      </c>
+      <c r="P70" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>630</v>
+      </c>
+      <c r="B71" t="s">
+        <v>631</v>
+      </c>
+      <c r="C71" t="s">
+        <v>624</v>
+      </c>
+      <c r="D71" t="s">
+        <v>625</v>
+      </c>
+      <c r="E71" t="s">
+        <v>28</v>
+      </c>
+      <c r="F71" t="s">
+        <v>47</v>
+      </c>
+      <c r="G71">
+        <v>30</v>
+      </c>
+      <c r="H71" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J71" t="s">
+        <v>632</v>
+      </c>
+      <c r="K71" t="b">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>379</v>
+      </c>
+      <c r="O71" t="s">
+        <v>600</v>
+      </c>
+      <c r="P71" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>633</v>
+      </c>
+      <c r="B72" t="s">
+        <v>634</v>
+      </c>
+      <c r="C72" t="s">
+        <v>624</v>
+      </c>
+      <c r="D72" t="s">
+        <v>625</v>
+      </c>
+      <c r="E72" t="s">
+        <v>47</v>
+      </c>
+      <c r="F72" t="s">
+        <v>89</v>
+      </c>
+      <c r="G72">
+        <v>30</v>
+      </c>
+      <c r="H72" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J72" t="s">
+        <v>635</v>
+      </c>
+      <c r="K72" t="b">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>505</v>
+      </c>
+      <c r="O72" t="s">
+        <v>600</v>
+      </c>
+      <c r="P72" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>636</v>
+      </c>
+      <c r="B73" t="s">
+        <v>637</v>
+      </c>
+      <c r="C73" t="s">
+        <v>624</v>
+      </c>
+      <c r="D73" t="s">
+        <v>625</v>
+      </c>
+      <c r="E73" t="s">
+        <v>47</v>
+      </c>
+      <c r="F73" t="s">
+        <v>89</v>
+      </c>
+      <c r="G73">
+        <v>30</v>
+      </c>
+      <c r="H73" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J73" t="s">
+        <v>638</v>
+      </c>
+      <c r="K73" t="b">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>505</v>
+      </c>
+      <c r="O73" t="s">
+        <v>600</v>
+      </c>
+      <c r="P73" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>639</v>
+      </c>
+      <c r="B74" t="s">
+        <v>640</v>
+      </c>
+      <c r="C74" t="s">
+        <v>624</v>
+      </c>
+      <c r="D74" t="s">
+        <v>625</v>
+      </c>
+      <c r="E74" t="s">
+        <v>47</v>
+      </c>
+      <c r="F74" t="s">
+        <v>89</v>
+      </c>
+      <c r="G74">
+        <v>30</v>
+      </c>
+      <c r="H74" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J74" t="s">
+        <v>641</v>
+      </c>
+      <c r="K74" t="b">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>505</v>
+      </c>
+      <c r="O74" t="s">
+        <v>600</v>
+      </c>
+      <c r="P74" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>642</v>
+      </c>
+      <c r="B75" t="s">
+        <v>643</v>
+      </c>
+      <c r="C75" t="s">
+        <v>624</v>
+      </c>
+      <c r="D75" t="s">
+        <v>625</v>
+      </c>
+      <c r="E75" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" t="s">
+        <v>66</v>
+      </c>
+      <c r="G75">
+        <v>30</v>
+      </c>
+      <c r="H75" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J75" t="s">
+        <v>644</v>
+      </c>
+      <c r="K75" t="b">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>505</v>
+      </c>
+      <c r="O75" t="s">
+        <v>600</v>
+      </c>
+      <c r="P75" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>645</v>
+      </c>
+      <c r="B76" t="s">
+        <v>646</v>
+      </c>
+      <c r="C76" t="s">
+        <v>624</v>
+      </c>
+      <c r="D76" t="s">
+        <v>625</v>
+      </c>
+      <c r="E76" t="s">
+        <v>47</v>
+      </c>
+      <c r="F76" t="s">
+        <v>66</v>
+      </c>
+      <c r="G76">
+        <v>30</v>
+      </c>
+      <c r="H76" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J76" t="s">
+        <v>647</v>
+      </c>
+      <c r="K76" t="b">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>505</v>
+      </c>
+      <c r="O76" t="s">
+        <v>600</v>
+      </c>
+      <c r="P76" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>648</v>
+      </c>
+      <c r="B77" t="s">
+        <v>649</v>
+      </c>
+      <c r="C77" t="s">
+        <v>624</v>
+      </c>
+      <c r="D77" t="s">
+        <v>625</v>
+      </c>
+      <c r="E77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77">
+        <v>30</v>
+      </c>
+      <c r="H77" s="3">
+        <v>43217</v>
+      </c>
+      <c r="J77" t="s">
+        <v>650</v>
+      </c>
+      <c r="K77" t="b">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>505</v>
+      </c>
+      <c r="O77" t="s">
+        <v>600</v>
+      </c>
+      <c r="P77" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>676</v>
+      </c>
+      <c r="B78" t="s">
+        <v>677</v>
+      </c>
+      <c r="C78" t="s">
+        <v>624</v>
+      </c>
+      <c r="D78" t="s">
+        <v>678</v>
+      </c>
+      <c r="E78" t="s">
+        <v>66</v>
+      </c>
+      <c r="F78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G78">
+        <v>30</v>
+      </c>
+      <c r="H78" s="3">
+        <v>43203</v>
+      </c>
+      <c r="J78" t="s">
+        <v>679</v>
+      </c>
+      <c r="K78" t="b">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="O78" t="s">
+        <v>600</v>
+      </c>
+      <c r="P78" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>680</v>
+      </c>
+      <c r="B79" t="s">
+        <v>681</v>
+      </c>
+      <c r="C79" t="s">
+        <v>624</v>
+      </c>
+      <c r="E79" t="s">
+        <v>66</v>
+      </c>
+      <c r="F79" t="s">
+        <v>89</v>
+      </c>
+      <c r="G79">
+        <v>30</v>
+      </c>
+      <c r="H79" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J79" t="s">
+        <v>682</v>
+      </c>
+      <c r="K79" t="b">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>464</v>
+      </c>
+      <c r="O79" t="s">
+        <v>600</v>
+      </c>
+      <c r="P79" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>683</v>
+      </c>
+      <c r="B80" t="s">
+        <v>684</v>
+      </c>
+      <c r="C80" t="s">
+        <v>624</v>
+      </c>
+      <c r="E80" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80">
+        <v>30</v>
+      </c>
+      <c r="H80" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J80" t="s">
+        <v>685</v>
+      </c>
+      <c r="K80" t="b">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>379</v>
+      </c>
+      <c r="O80" t="s">
+        <v>600</v>
+      </c>
+      <c r="P80" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>686</v>
+      </c>
+      <c r="B81" t="s">
+        <v>687</v>
+      </c>
+      <c r="C81" t="s">
+        <v>624</v>
+      </c>
+      <c r="E81" t="s">
+        <v>47</v>
+      </c>
+      <c r="F81" t="s">
+        <v>89</v>
+      </c>
+      <c r="G81">
+        <v>30</v>
+      </c>
+      <c r="H81" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J81" t="s">
+        <v>688</v>
+      </c>
+      <c r="K81" t="b">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>464</v>
+      </c>
+      <c r="O81" t="s">
+        <v>600</v>
+      </c>
+      <c r="P81" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>689</v>
+      </c>
+      <c r="B82" t="s">
+        <v>690</v>
+      </c>
+      <c r="C82" t="s">
+        <v>624</v>
+      </c>
+      <c r="E82" t="s">
+        <v>52</v>
+      </c>
+      <c r="F82" t="s">
+        <v>71</v>
+      </c>
+      <c r="G82">
+        <v>30</v>
+      </c>
+      <c r="H82" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J82" t="s">
+        <v>691</v>
+      </c>
+      <c r="K82" t="b">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>379</v>
+      </c>
+      <c r="O82" t="s">
+        <v>600</v>
+      </c>
+      <c r="P82" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>692</v>
+      </c>
+      <c r="B83" t="s">
+        <v>693</v>
+      </c>
+      <c r="C83" t="s">
+        <v>624</v>
+      </c>
+      <c r="E83" t="s">
+        <v>71</v>
+      </c>
+      <c r="F83" t="s">
+        <v>89</v>
+      </c>
+      <c r="G83">
+        <v>30</v>
+      </c>
+      <c r="H83" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J83" t="s">
+        <v>694</v>
+      </c>
+      <c r="K83" t="b">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>464</v>
+      </c>
+      <c r="O83" t="s">
+        <v>600</v>
+      </c>
+      <c r="P83" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>695</v>
+      </c>
+      <c r="B84" t="s">
+        <v>696</v>
+      </c>
+      <c r="C84" t="s">
+        <v>624</v>
+      </c>
+      <c r="E84" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" t="s">
+        <v>47</v>
+      </c>
+      <c r="G84">
+        <v>30</v>
+      </c>
+      <c r="H84" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J84" t="s">
+        <v>697</v>
+      </c>
+      <c r="K84" t="b">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>379</v>
+      </c>
+      <c r="O84" t="s">
+        <v>600</v>
+      </c>
+      <c r="P84" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>698</v>
+      </c>
+      <c r="B85" t="s">
+        <v>699</v>
+      </c>
+      <c r="C85" t="s">
+        <v>624</v>
+      </c>
+      <c r="E85" t="s">
+        <v>47</v>
+      </c>
+      <c r="F85" t="s">
+        <v>89</v>
+      </c>
+      <c r="G85">
+        <v>30</v>
+      </c>
+      <c r="H85" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J85" t="s">
+        <v>700</v>
+      </c>
+      <c r="K85" t="b">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>464</v>
+      </c>
+      <c r="O85" t="s">
+        <v>600</v>
+      </c>
+      <c r="P85" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>701</v>
+      </c>
+      <c r="B86" t="s">
+        <v>702</v>
+      </c>
+      <c r="C86" t="s">
+        <v>624</v>
+      </c>
+      <c r="E86" t="s">
+        <v>52</v>
+      </c>
+      <c r="F86" t="s">
+        <v>71</v>
+      </c>
+      <c r="G86">
+        <v>30</v>
+      </c>
+      <c r="H86" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J86" t="s">
+        <v>703</v>
+      </c>
+      <c r="K86" t="b">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <v>379</v>
+      </c>
+      <c r="O86" t="s">
+        <v>600</v>
+      </c>
+      <c r="P86" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>704</v>
+      </c>
+      <c r="B87" t="s">
+        <v>705</v>
+      </c>
+      <c r="C87" t="s">
+        <v>624</v>
+      </c>
+      <c r="E87" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" t="s">
+        <v>89</v>
+      </c>
+      <c r="G87">
+        <v>30</v>
+      </c>
+      <c r="H87" s="3">
+        <v>43224</v>
+      </c>
+      <c r="J87" t="s">
+        <v>706</v>
+      </c>
+      <c r="K87" t="b">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>464</v>
+      </c>
+      <c r="O87" t="s">
+        <v>600</v>
+      </c>
+      <c r="P87" t="s">
         <v>881</v>
       </c>
     </row>
@@ -14157,6 +15020,198 @@
     <mergeCell ref="C38:D38"/>
   </mergeCells>
   <conditionalFormatting sqref="O1:P1">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O23:O34 O20:O21">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:O34">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -14168,7 +15223,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O23:O34 O20:O21">
+  <conditionalFormatting sqref="O3">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -14180,7 +15235,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O20:O34">
+  <conditionalFormatting sqref="O3">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -14192,7 +15247,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
+  <conditionalFormatting sqref="O2">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -14204,7 +15259,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
+  <conditionalFormatting sqref="O2">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -14216,7 +15271,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
+  <conditionalFormatting sqref="O35:O38">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -14228,7 +15283,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
+  <conditionalFormatting sqref="O35:O38">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -14240,7 +15295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8">
+  <conditionalFormatting sqref="O39:O41">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -14252,7 +15307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8">
+  <conditionalFormatting sqref="O39:O41">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -14264,7 +15319,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O7">
+  <conditionalFormatting sqref="O56:O68">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -14276,7 +15331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O7">
+  <conditionalFormatting sqref="O56:O68">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -14288,175 +15343,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O6">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O6">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O35:O38">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O35:O38">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O39:O41">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O39:O41">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O56:O68">
+  <conditionalFormatting sqref="O69:O87">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -14468,7 +15355,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O56:O68">
+  <conditionalFormatting sqref="O69:O87">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -14488,8 +15375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>